<commit_message>
Documents Update adding estimation and some Devops env. tools
</commit_message>
<xml_diff>
--- a/Management/CrowSoft Costing Document.xlsx
+++ b/Management/CrowSoft Costing Document.xlsx
@@ -618,7 +618,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -629,7 +629,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updating Sprint0 Cost document and adding Sprint 0 report
</commit_message>
<xml_diff>
--- a/Management/CrowSoft Costing Document.xlsx
+++ b/Management/CrowSoft Costing Document.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12510" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Resources" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="63">
   <si>
     <t>Colin Kenny</t>
   </si>
@@ -120,113 +120,104 @@
     <t xml:space="preserve">dev </t>
   </si>
   <si>
-    <t>Server Name opt/CJknSvr</t>
-  </si>
-  <si>
     <t>Server Name opt/Csft_dev</t>
   </si>
   <si>
-    <t>Dev-stage-Prod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Server Name </t>
-  </si>
-  <si>
     <t>OS</t>
   </si>
   <si>
     <t>Ubuntu 16.04</t>
   </si>
   <si>
-    <t xml:space="preserve">Windows </t>
-  </si>
-  <si>
     <t xml:space="preserve">Hosting </t>
   </si>
   <si>
-    <t xml:space="preserve">Web Application </t>
-  </si>
-  <si>
-    <t>UI Component</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DB -- TBD </t>
-  </si>
-  <si>
-    <t>Server Name C:/Path</t>
-  </si>
-  <si>
     <t>Cost Per Year</t>
   </si>
   <si>
-    <t>Continious Integration suite</t>
-  </si>
-  <si>
     <t>Weely Hours</t>
   </si>
   <si>
     <t xml:space="preserve">Cost </t>
   </si>
   <si>
+    <t>CS000001</t>
+  </si>
+  <si>
+    <t>CS000002</t>
+  </si>
+  <si>
+    <t>CS000003</t>
+  </si>
+  <si>
+    <t>Work ID</t>
+  </si>
+  <si>
+    <t>CS000004</t>
+  </si>
+  <si>
+    <t>CS000005</t>
+  </si>
+  <si>
+    <t>CS000006</t>
+  </si>
+  <si>
+    <t>CS000007</t>
+  </si>
+  <si>
+    <t>CS000008</t>
+  </si>
+  <si>
+    <t>CS000009</t>
+  </si>
+  <si>
+    <t>CS000001@crowsoft.ie</t>
+  </si>
+  <si>
+    <t>CS000002@crowsoft.ie</t>
+  </si>
+  <si>
+    <t>CS000003@crowsoft.ie</t>
+  </si>
+  <si>
+    <t>CS000004@crowsoft.ie</t>
+  </si>
+  <si>
+    <t>CS000005@crowsoft.ie</t>
+  </si>
+  <si>
+    <t>CS000006@crowsoft.ie</t>
+  </si>
+  <si>
+    <t>CS000007@crowsoft.ie</t>
+  </si>
+  <si>
+    <t>CS000008@crowsoft.ie</t>
+  </si>
+  <si>
+    <t>CS000009@crowsoft.ie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total </t>
+  </si>
+  <si>
+    <t>Developer/Engineer</t>
+  </si>
+  <si>
+    <t>Web Application &amp; DB</t>
+  </si>
+  <si>
+    <t>Server Name opt/CSJknSvr</t>
+  </si>
+  <si>
+    <t>DEV-Stage-Prod</t>
+  </si>
+  <si>
+    <t>Jenkins Server - Continious Integration suite</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sprint 1
-Building test environment - Application Development - </t>
-  </si>
-  <si>
-    <t>CS000001</t>
-  </si>
-  <si>
-    <t>CS000002</t>
-  </si>
-  <si>
-    <t>CS000003</t>
-  </si>
-  <si>
-    <t>Work ID</t>
-  </si>
-  <si>
-    <t>CS000004</t>
-  </si>
-  <si>
-    <t>CS000005</t>
-  </si>
-  <si>
-    <t>CS000006</t>
-  </si>
-  <si>
-    <t>CS000007</t>
-  </si>
-  <si>
-    <t>CS000008</t>
-  </si>
-  <si>
-    <t>CS000009</t>
-  </si>
-  <si>
-    <t>CS000001@crowsoft.ie</t>
-  </si>
-  <si>
-    <t>CS000002@crowsoft.ie</t>
-  </si>
-  <si>
-    <t>CS000003@crowsoft.ie</t>
-  </si>
-  <si>
-    <t>CS000004@crowsoft.ie</t>
-  </si>
-  <si>
-    <t>CS000005@crowsoft.ie</t>
-  </si>
-  <si>
-    <t>CS000006@crowsoft.ie</t>
-  </si>
-  <si>
-    <t>CS000007@crowsoft.ie</t>
-  </si>
-  <si>
-    <t>CS000008@crowsoft.ie</t>
-  </si>
-  <si>
-    <t>CS000009@crowsoft.ie</t>
+Building Development  environment </t>
   </si>
 </sst>
 </file>
@@ -250,7 +241,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -275,6 +266,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -289,7 +286,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -311,6 +308,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -618,7 +621,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -628,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,7 +640,8 @@
     <col min="1" max="1" width="27.140625" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="4" max="5" width="18" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
     <col min="6" max="6" width="16.28515625" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="32.140625" customWidth="1"/>
@@ -648,7 +652,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -671,10 +675,10 @@
         <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -690,13 +694,16 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -704,13 +711,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="D4" t="s">
         <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -718,13 +728,16 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -732,13 +745,16 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
         <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -746,13 +762,16 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -760,13 +779,16 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
         <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -774,13 +796,16 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -788,13 +813,16 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
         <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -818,10 +846,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,13 +867,13 @@
       <c r="D1" s="9"/>
     </row>
     <row r="2" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8" t="s">
-        <v>45</v>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -863,6 +891,9 @@
       <c r="B4">
         <v>10</v>
       </c>
+      <c r="D4" s="11">
+        <v>500</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -871,6 +902,9 @@
       <c r="B5">
         <v>10</v>
       </c>
+      <c r="D5" s="11">
+        <v>500</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -879,6 +913,9 @@
       <c r="B6">
         <v>10</v>
       </c>
+      <c r="D6" s="11">
+        <v>500</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -887,6 +924,9 @@
       <c r="B7">
         <v>10</v>
       </c>
+      <c r="D7" s="11">
+        <v>500</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -895,6 +935,9 @@
       <c r="B8">
         <v>10</v>
       </c>
+      <c r="D8" s="11">
+        <v>500</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -903,6 +946,9 @@
       <c r="B9">
         <v>10</v>
       </c>
+      <c r="D9" s="11">
+        <v>500</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -911,52 +957,65 @@
       <c r="B10">
         <v>10</v>
       </c>
+      <c r="D10" s="11">
+        <v>500</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8" t="s">
-        <v>45</v>
-      </c>
+      <c r="B11" s="13">
+        <v>10</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="13">
+        <f>SUM(B3:B11)</f>
+        <v>80</v>
+      </c>
+      <c r="C12" s="13"/>
+      <c r="D12" s="14">
+        <f>SUM(D4:D11)</f>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16">
-        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B17">
         <v>10</v>
@@ -964,7 +1023,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B18">
         <v>10</v>
@@ -972,7 +1031,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B19">
         <v>10</v>
@@ -980,7 +1039,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B20">
         <v>10</v>
@@ -988,7 +1047,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B21">
         <v>10</v>
@@ -996,7 +1055,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B22">
         <v>10</v>
@@ -1004,18 +1063,27 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="B23">
+      <c r="B24">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A14:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1024,7 +1092,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,8 +1100,8 @@
     <col min="1" max="1" width="32.42578125" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1053,27 +1121,27 @@
         <v>28</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
         <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="E3" s="7">
         <v>3500</v>
@@ -1081,56 +1149,25 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="E4" s="7">
         <v>3500</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="7">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
+      <c r="E5" s="7"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" t="s">
-        <v>43</v>
-      </c>
       <c r="E10" s="7">
         <v>3500</v>
       </c>

</xml_diff>

<commit_message>
updated VMWare document to include jenkins integration with github
</commit_message>
<xml_diff>
--- a/Management/CrowSoft Costing Document.xlsx
+++ b/Management/CrowSoft Costing Document.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="63">
   <si>
     <t>Colin Kenny</t>
   </si>
@@ -302,18 +302,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -621,7 +621,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -846,10 +846,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,20 +859,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="2" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10" t="s">
         <v>36</v>
       </c>
     </row>
@@ -891,7 +891,7 @@
       <c r="B4">
         <v>10</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="9">
         <v>500</v>
       </c>
     </row>
@@ -902,7 +902,7 @@
       <c r="B5">
         <v>10</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="9">
         <v>500</v>
       </c>
     </row>
@@ -913,7 +913,7 @@
       <c r="B6">
         <v>10</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="9">
         <v>500</v>
       </c>
     </row>
@@ -924,7 +924,7 @@
       <c r="B7">
         <v>10</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="9">
         <v>500</v>
       </c>
     </row>
@@ -935,7 +935,7 @@
       <c r="B8">
         <v>10</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="9">
         <v>500</v>
       </c>
     </row>
@@ -946,7 +946,7 @@
       <c r="B9">
         <v>10</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="9">
         <v>500</v>
       </c>
     </row>
@@ -957,43 +957,43 @@
       <c r="B10">
         <v>10</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="9">
         <v>500</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="13">
-        <v>10</v>
-      </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="14">
+      <c r="B11" s="11">
+        <v>10</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12">
         <v>500</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12" s="11">
         <f>SUM(B3:B11)</f>
         <v>80</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="14">
+      <c r="C12" s="11"/>
+      <c r="D12" s="12">
         <f>SUM(D4:D11)</f>
         <v>4000</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
@@ -1013,68 +1013,106 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
       <c r="B17">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D17" s="9">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
       <c r="B18">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D18" s="9">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
       <c r="B19">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D19" s="9">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
       <c r="B20">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D20" s="9">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
       <c r="B21">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D21" s="9">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>14</v>
       </c>
       <c r="B22">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D22" s="9">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
       <c r="B23">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D23" s="9">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24">
         <v>10</v>
+      </c>
+      <c r="D24" s="12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="11">
+        <f>SUM(B16:B24)</f>
+        <v>80</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="12">
+        <f>SUM(D17:D24)</f>
+        <v>4000</v>
       </c>
     </row>
   </sheetData>
@@ -1105,13 +1143,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">

</xml_diff>